<commit_message>
reverted agenda.py and agenda_test.py to simple commandline version. And removed all other files.
</commit_message>
<xml_diff>
--- a/agenda_output.xlsx
+++ b/agenda_output.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Duration</t>
+          <t>60</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Introduction</t>
+          <t>Intro</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">

</xml_diff>

<commit_message>
finished import and export to excel functions. And main function. Need to tidy up commented out lines etc
</commit_message>
<xml_diff>
--- a/agenda_output.xlsx
+++ b/agenda_output.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>Duration</t>
         </is>
       </c>
     </row>
@@ -459,17 +459,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10:15:00</t>
+          <t>10:25:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Intro</t>
+          <t>Topic 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>25</t>
         </is>
       </c>
     </row>
@@ -479,22 +479,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10:15:00</t>
+          <t>10:25:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11:00:00</t>
+          <t>10:55:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Topic 1</t>
+          <t>Topic 2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>30</t>
         </is>
       </c>
     </row>
@@ -504,22 +504,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11:00:00</t>
+          <t>10:55:00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>11:25:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Topic 2</t>
+          <t>Break</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>30</t>
         </is>
       </c>
     </row>
@@ -529,22 +529,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>11:25:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12:15:00</t>
+          <t>11:45:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Break</t>
+          <t>Topic 3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
     </row>
@@ -554,22 +554,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12:15:00</t>
+          <t>11:45:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>12:40:00</t>
+          <t>12:45:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Topic 3</t>
+          <t>Topic 4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>60</t>
         </is>
       </c>
     </row>
@@ -579,22 +579,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12:40:00</t>
+          <t>12:45:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>13:25:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Topic 4</t>
+          <t>Break</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>15</t>
         </is>
       </c>
     </row>
@@ -604,22 +604,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>13:25:00</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>14:25:00</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Topic 5</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>25</t>
         </is>
       </c>
     </row>
@@ -629,22 +629,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14:25:00</t>
+          <t>13:25:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>16:25:00</t>
+          <t>13:55:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Topic 5</t>
+          <t>Topic 6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>30</t>
         </is>
       </c>
     </row>
@@ -654,22 +654,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16:25:00</t>
+          <t>13:55:00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>17:25:00</t>
+          <t>14:40:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Topic 6</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>45</t>
         </is>
       </c>
     </row>
@@ -679,22 +679,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17:25:00</t>
+          <t>14:40:00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>17:40:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Closing</t>
+          <t>Topic 7</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
     </row>

</xml_diff>